<commit_message>
Stop the refreshing of value, to write something
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -10,12 +10,15 @@
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$14</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Priority</t>
   </si>
@@ -120,6 +123,9 @@
   </si>
   <si>
     <t>to watch the different problem from application</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -210,7 +216,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -224,105 +230,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -644,11 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuil1"/>
+  <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -686,7 +594,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -735,7 +643,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -753,7 +661,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -789,7 +697,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -807,7 +715,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -825,7 +733,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
@@ -843,7 +751,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -861,7 +769,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
@@ -879,7 +787,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1586,6 +1494,13 @@
       <c r="G100" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="B2:C14">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="To do"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="B3:B100">
     <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Medium"</formula>
@@ -1598,13 +1513,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C100">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Search of variable without lag
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Priority</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>To test</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -684,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Issue with boucle to avoid the lag
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Priority</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>In progress</t>
-  </si>
-  <si>
-    <t>To test</t>
   </si>
 </sst>
 </file>
@@ -687,7 +684,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Correct issue with timer to wait the text writing.
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -556,7 +556,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -679,12 +679,12 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>19</v>
@@ -1497,6 +1497,7 @@
   <autoFilter ref="B2:C14">
     <filterColumn colId="1">
       <filters>
+        <filter val="In progress"/>
         <filter val="To do"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Now Force variable is  possible
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Priority</t>
   </si>
@@ -125,7 +125,13 @@
     <t>to watch the different problem from application</t>
   </si>
   <si>
-    <t>In progress</t>
+    <t>To test</t>
+  </si>
+  <si>
+    <t>to write the value of variable</t>
+  </si>
+  <si>
+    <t>to change the variable 's value</t>
   </si>
 </sst>
 </file>
@@ -556,7 +562,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -612,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -806,11 +812,21 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Writting of Interger variable
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -562,7 +562,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -816,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Starting of time stamp at unix format, actually the format is a long type
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -41,9 +41,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>To do</t>
-  </si>
-  <si>
     <t>to force of variables</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>to change the variable 's value</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -600,13 +600,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="F3" s="4">
         <v>10</v>
@@ -618,13 +618,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F4" s="4">
         <v>5</v>
@@ -633,16 +633,16 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -654,13 +654,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="4">
         <v>5</v>
@@ -672,13 +672,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="4">
         <v>3</v>
@@ -687,16 +687,16 @@
     </row>
     <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
@@ -708,13 +708,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F9" s="4">
         <v>4</v>
@@ -726,13 +726,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F10" s="4">
         <v>4</v>
@@ -741,16 +741,16 @@
     </row>
     <row r="11" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
@@ -762,13 +762,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="4">
         <v>4</v>
@@ -780,13 +780,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="4">
         <v>3</v>
@@ -795,16 +795,16 @@
     </row>
     <row r="14" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -816,13 +816,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
New functionality to implement
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Priority</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>to change the variable 's value</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>to import all variable</t>
+  </si>
+  <si>
+    <t>to unlock the treatment of variable in U-Test</t>
   </si>
 </sst>
 </file>
@@ -559,7 +568,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -827,11 +836,21 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New magic button to import all variable, thus we can listen all variables. This temporary magic button unlock U-Test :).
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>Priority</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>to change the variable 's value</t>
-  </si>
-  <si>
-    <t>To do</t>
   </si>
   <si>
     <t>to import all variable</t>
@@ -568,7 +565,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -840,13 +837,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Add some elements to do improving the tool
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$17</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>Priority</t>
   </si>
@@ -135,6 +135,33 @@
   </si>
   <si>
     <t>to unlock the treatment of variable in U-Test</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>to have a checkbox (or toogle button)</t>
+  </si>
+  <si>
+    <t>to modify the write's type (force or write)</t>
+  </si>
+  <si>
+    <t>to put the maximum number</t>
+  </si>
+  <si>
+    <t>to display more or less variable</t>
+  </si>
+  <si>
+    <t>to be able to put regular expression in search field</t>
+  </si>
+  <si>
+    <t>to improve the search</t>
+  </si>
+  <si>
+    <t>to improve the variable's visibility</t>
+  </si>
+  <si>
+    <t>to display more variables</t>
   </si>
 </sst>
 </file>
@@ -565,7 +592,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -634,7 +661,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
@@ -832,7 +859,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -851,35 +878,75 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2</v>
+      </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="4">
+        <v>4</v>
+      </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4</v>
+      </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -1523,11 +1590,11 @@
       <c r="G100" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:C14">
+  <autoFilter ref="B2:C17">
     <filterColumn colId="1">
       <filters>
-        <filter val="In progress"/>
         <filter val="To do"/>
+        <filter val="To test"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Integration of type in DataObserver (Integer, Double...)
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -592,7 +592,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -882,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Writing on double variable
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -592,7 +592,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -846,7 +846,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Add of new functionality
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>Priority</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>to display more variables</t>
+  </si>
+  <si>
+    <t>to have a log file</t>
+  </si>
+  <si>
+    <t>to see the diffrent application error</t>
   </si>
 </sst>
 </file>
@@ -592,7 +598,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -950,10 +956,18 @@
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="3"/>
     </row>

</xml_diff>

<commit_message>
New functionalities to perform
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>Priority</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>to see the diffrent application error</t>
+  </si>
+  <si>
+    <t>to check or not the copyboard</t>
+  </si>
+  <si>
+    <t>to avoid removing the search</t>
   </si>
 </sst>
 </file>
@@ -598,7 +604,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -915,13 +921,13 @@
         <v>43</v>
       </c>
       <c r="F18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>39</v>
@@ -957,7 +963,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>39</v>
@@ -968,15 +974,27 @@
       <c r="E21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="4">
+        <v>4</v>
+      </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
The number of visible variable is customizable
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$22</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -604,7 +604,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
@@ -907,12 +907,12 @@
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>42</v>
@@ -1622,7 +1622,7 @@
       <c r="G100" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:C17">
+  <autoFilter ref="B2:C22">
     <filterColumn colId="1">
       <filters>
         <filter val="To do"/>

</xml_diff>

<commit_message>
The clipboard checking can be disabled. The width of column are in "Auto" value. The search filed shouldn't accepted the newline anymore.
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -604,7 +604,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -979,12 +979,12 @@
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Add of one functionality in Work file (copy the entirely name when we copy the path field value in dashboard)
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>Priority</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>to avoid removing the search</t>
+  </si>
+  <si>
+    <t>to copy the path and name when we copy the path field</t>
+  </si>
+  <si>
+    <t>to have directly the whole variable</t>
   </si>
 </sst>
 </file>
@@ -604,13 +610,13 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="13.7109375"/>
-    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875"/>
@@ -998,11 +1004,21 @@
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New functionality to copy the path and name directly when we just copy  the path
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -176,10 +176,10 @@
     <t>to avoid removing the search</t>
   </si>
   <si>
-    <t>to copy the path and name when we copy the path field</t>
-  </si>
-  <si>
-    <t>to have directly the whole variable</t>
+    <t>to copy the path and name when we are in the path column</t>
+  </si>
+  <si>
+    <t>to have directly the path and name</t>
   </si>
 </sst>
 </file>
@@ -610,13 +610,13 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="13.7109375"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875"/>

</xml_diff>

<commit_message>
The Regex works. The old search has been replaced by the regex search
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>Priority</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>to have directly the path and name</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -610,7 +613,7 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -936,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Regex choice has been implemented.
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>Priority</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>to have directly the path and name</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -939,7 +936,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
The regex search shouldn't crash anymore. Add some functionalities.
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$25</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>Priority</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>to have directly the path and name</t>
+  </si>
+  <si>
+    <t>to set a list of variable with a color associated at a value</t>
+  </si>
+  <si>
+    <t>to display the good value or wrong value direclty in background</t>
+  </si>
+  <si>
+    <t>to set a search background color when the regex is wrong or good</t>
+  </si>
+  <si>
+    <t>to see whether the regex has worked</t>
   </si>
 </sst>
 </file>
@@ -259,7 +271,55 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -610,14 +670,14 @@
   <dimension ref="B2:G100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="13.7109375"/>
-    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875"/>
     <col min="8" max="1026" width="11.5703125"/>
@@ -895,12 +955,12 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>40</v>
@@ -951,19 +1011,19 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F20" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -1022,19 +1082,39 @@
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="4">
+        <v>4</v>
+      </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -1638,7 +1718,7 @@
       <c r="G100" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:C22">
+  <autoFilter ref="B2:C25">
     <filterColumn colId="1">
       <filters>
         <filter val="To do"/>
@@ -1646,28 +1726,32 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState ref="B3:G25">
+    <sortCondition sortBy="cellColor" ref="B3:B25" dxfId="3"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="B3:B25" dxfId="2"/>
+  </sortState>
   <conditionalFormatting sqref="B3:B100">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C100">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add some functionalities in the requirement file
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
   <si>
     <t>Priority</t>
   </si>
@@ -192,6 +192,27 @@
   </si>
   <si>
     <t>to see whether the regex has worked</t>
+  </si>
+  <si>
+    <t>Real (hours)</t>
+  </si>
+  <si>
+    <t>the locked list are automatically saved</t>
+  </si>
+  <si>
+    <t>to load automatically the locked list and the application shouldn't carsh</t>
+  </si>
+  <si>
+    <t>to display the information in a status bar</t>
+  </si>
+  <si>
+    <t>for the messages doesn't alter the size</t>
+  </si>
+  <si>
+    <t>to save as a list of locked variable</t>
+  </si>
+  <si>
+    <t>to load quicly a list of locked elements</t>
   </si>
 </sst>
 </file>
@@ -271,7 +292,120 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -317,55 +451,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -667,23 +752,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1" filterMode="1"/>
-  <dimension ref="B2:G100"/>
+  <dimension ref="B2:H100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="13.7109375"/>
     <col min="4" max="4" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875"/>
-    <col min="8" max="1026" width="11.5703125"/>
+    <col min="7" max="7" width="15.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875"/>
+    <col min="9" max="1027" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -700,10 +786,13 @@
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -719,9 +808,12 @@
       <c r="F3" s="4">
         <v>10</v>
       </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -737,27 +829,33 @@
       <c r="F4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F5" s="4">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -765,17 +863,20 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -783,35 +884,41 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F7" s="4">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -819,17 +926,20 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4">
         <v>4</v>
       </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="4">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -837,35 +947,41 @@
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F10" s="4">
-        <v>4</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -873,17 +989,20 @@
         <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4">
-        <v>4</v>
-      </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
@@ -891,71 +1010,81 @@
         <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F13" s="4">
-        <v>3</v>
-      </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F14" s="4">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F15" s="4">
-        <v>1</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="G15" s="4">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -963,71 +1092,83 @@
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
       </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4">
-        <v>4</v>
-      </c>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F20" s="4">
-        <v>10</v>
-      </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1043,27 +1184,29 @@
       <c r="F21" s="4">
         <v>4</v>
       </c>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="4"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F22" s="4">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1071,651 +1214,761 @@
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="4">
         <v>2</v>
       </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+      <c r="G24" s="4">
+        <v>2</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="4">
+        <v>3</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F26" s="4">
         <v>4</v>
       </c>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="4"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="4"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="4"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="4"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="4"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="4"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="4"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="4"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="4"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="4"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="4"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="4"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="4"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="4"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="4"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="4"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="4"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="4"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="4"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="4"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="4"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="4"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="4"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="4"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="4"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="4"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G54" s="4"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="3"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G55" s="4"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="3"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="4"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="3"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="4"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G58" s="4"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="3"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G59" s="4"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="4"/>
-      <c r="G60" s="3"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G60" s="4"/>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="3"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G61" s="4"/>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="4"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G63" s="4"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="3"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="4"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="4"/>
-      <c r="G65" s="3"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G65" s="4"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="4"/>
-      <c r="G66" s="3"/>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="4"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="3"/>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="4"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G68" s="4"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="4"/>
-      <c r="G69" s="3"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G69" s="4"/>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="4"/>
-      <c r="G70" s="3"/>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G70" s="4"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="4"/>
-      <c r="G71" s="3"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G71" s="4"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="4"/>
-      <c r="G72" s="3"/>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G72" s="4"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="4"/>
-      <c r="G73" s="3"/>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G73" s="4"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="3"/>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G74" s="4"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="3"/>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G75" s="4"/>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="3"/>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G76" s="4"/>
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="3"/>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G77" s="4"/>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G78" s="4"/>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="4"/>
-      <c r="G79" s="3"/>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G79" s="4"/>
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="3"/>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G80" s="4"/>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="4"/>
-      <c r="G81" s="3"/>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G81" s="4"/>
+      <c r="H81" s="3"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G82" s="4"/>
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G83" s="4"/>
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="4"/>
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G84" s="4"/>
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="4"/>
-      <c r="G85" s="3"/>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G85" s="4"/>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="3"/>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G86" s="4"/>
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="4"/>
-      <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G87" s="4"/>
+      <c r="H87" s="3"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="4"/>
-      <c r="G88" s="3"/>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G88" s="4"/>
+      <c r="H88" s="3"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="4"/>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G89" s="4"/>
+      <c r="H89" s="3"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="4"/>
-      <c r="G90" s="3"/>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G90" s="4"/>
+      <c r="H90" s="3"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="4"/>
-      <c r="G91" s="3"/>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G91" s="4"/>
+      <c r="H91" s="3"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="4"/>
-      <c r="G92" s="3"/>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G92" s="4"/>
+      <c r="H92" s="3"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="4"/>
-      <c r="G93" s="3"/>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G93" s="4"/>
+      <c r="H93" s="3"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="4"/>
-      <c r="G94" s="3"/>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G94" s="4"/>
+      <c r="H94" s="3"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="4"/>
-      <c r="G95" s="3"/>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G95" s="4"/>
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="4"/>
-      <c r="G96" s="3"/>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G96" s="4"/>
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="3"/>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G97" s="4"/>
+      <c r="H97" s="3"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="4"/>
-      <c r="G98" s="3"/>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G98" s="4"/>
+      <c r="H98" s="3"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="4"/>
-      <c r="G99" s="3"/>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G99" s="4"/>
+      <c r="H99" s="3"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="4"/>
-      <c r="G100" s="3"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:C25">
@@ -1726,33 +1979,33 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="B3:G25">
-    <sortCondition sortBy="cellColor" ref="B3:B25" dxfId="3"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="B3:B25" dxfId="2"/>
+  <sortState ref="B3:H28">
+    <sortCondition sortBy="cellColor" ref="B3:B28" dxfId="3"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="B3:B28" dxfId="2"/>
   </sortState>
   <conditionalFormatting sqref="B3:B100">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C100">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
-      <formula>"To do"</formula>
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"To test"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"To test"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
-      <formula>"Done"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Verification of the XML file structure, thus we can check whether the XML is correct
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>Priority</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>to load quicly a list of locked elements</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -292,71 +295,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -410,38 +349,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -755,7 +662,7 @@
   <dimension ref="B2:H100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1070,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>54</v>
@@ -1980,31 +1887,31 @@
     </filterColumn>
   </autoFilter>
   <sortState ref="B3:H28">
-    <sortCondition sortBy="cellColor" ref="B3:B28" dxfId="3"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="B3:B28" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="B3:B28" dxfId="8"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="B3:B28" dxfId="7"/>
   </sortState>
   <conditionalFormatting sqref="B3:B100">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C100">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ticket #5 : Implementing colors Add some comments and center the value of variable
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
   <si>
     <t>Priority</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>to load quicly a list of locked elements</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -662,7 +659,7 @@
   <dimension ref="B2:H100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -977,7 +974,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>54</v>
@@ -988,7 +985,9 @@
       <c r="F16" s="4">
         <v>10</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4">
+        <v>9</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add ID in Works excel file to identify each backlog's element
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$B$2:$C$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$C$2:$D$25</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>Priority</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>to load quicly a list of locked elements</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,11 +291,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -656,1228 +678,1348 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1" filterMode="1"/>
-  <dimension ref="B2:H100"/>
+  <dimension ref="B2:I100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="13.7109375"/>
-    <col min="4" max="4" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875"/>
-    <col min="9" max="1027" width="11.5703125"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875"/>
+    <col min="10" max="1028" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="6">
+        <f>ROW()</f>
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>10</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>5</v>
       </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="6">
+        <f>ROW()</f>
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5</v>
       </c>
       <c r="G5" s="4">
         <v>5</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="H5" s="4">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>3</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>1</v>
       </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>4</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>2</v>
       </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>4</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>3</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F9" s="4">
-        <v>4</v>
       </c>
       <c r="G9" s="4">
         <v>4</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="H9" s="4">
+        <v>4</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>3</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>2</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>2</v>
       </c>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
       </c>
       <c r="G12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="6">
+        <f>ROW()</f>
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F15" s="4">
-        <v>4</v>
       </c>
       <c r="G15" s="4">
         <v>4</v>
       </c>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+      <c r="H15" s="4">
+        <v>4</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="6">
+        <f>ROW()</f>
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>10</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>9</v>
       </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>2</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>5</v>
       </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>3</v>
       </c>
-      <c r="G19" s="4">
+      <c r="H19" s="4">
         <v>2</v>
       </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="F20" s="4">
-        <v>2</v>
       </c>
       <c r="G20" s="4">
         <v>2</v>
       </c>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
+      <c r="H20" s="4">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="6">
+        <f>ROW()</f>
+        <v>21</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>4</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="H21" s="4"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="6">
+        <f>ROW()</f>
+        <v>22</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="4">
+      <c r="G22" s="4">
         <v>2</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
+      <c r="H22" s="4"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="6">
+        <f>ROW()</f>
+        <v>23</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+      <c r="H23" s="4"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="F24" s="4">
-        <v>2</v>
       </c>
       <c r="G24" s="4">
         <v>2</v>
       </c>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+      <c r="H24" s="4">
+        <v>2</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="6">
+        <f>ROW()</f>
+        <v>25</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="4">
+      <c r="G25" s="4">
         <v>3</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+      <c r="H25" s="4"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="6">
+        <f>ROW()</f>
+        <v>26</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G26" s="4">
         <v>4</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+      <c r="H26" s="4"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="6">
+        <f>ROW()</f>
+        <v>27</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
         <v>1</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
+      <c r="H27" s="4"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="6">
+        <f>ROW()</f>
+        <v>28</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="4">
+      <c r="G28" s="4">
         <v>3</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="2"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="6"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="2"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="6"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
+      <c r="D30" s="2"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="2"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="6"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="2"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="6"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="2"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="2"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="6"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="2"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="2"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="6"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="3"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="2"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="6"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="2"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="6"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
+      <c r="D36" s="2"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
+      <c r="F36" s="3"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="2"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="6"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
+      <c r="F37" s="3"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="2"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="6"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
+      <c r="D38" s="2"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
+      <c r="F38" s="3"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="6"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="2"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="2"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="6"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="2"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
+      <c r="F40" s="3"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="2"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="6"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
+      <c r="F41" s="3"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="2"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="6"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="3"/>
+      <c r="D42" s="2"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
+      <c r="F42" s="3"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="2"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="6"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="2"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
+      <c r="F43" s="3"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="2"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="6"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="2"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
+      <c r="F44" s="3"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="2"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="6"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="2"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="6"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
+      <c r="D46" s="2"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
+      <c r="F46" s="3"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="2"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="6"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="2"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
+      <c r="F47" s="3"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="2"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="6"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
+      <c r="D48" s="2"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
+      <c r="F48" s="3"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="2"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="3"/>
+      <c r="D49" s="2"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
+      <c r="F49" s="3"/>
       <c r="G49" s="4"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="2"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B50" s="6"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="3"/>
+      <c r="D50" s="2"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
+      <c r="F50" s="3"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="2"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51" s="6"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="3"/>
+      <c r="D51" s="2"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
+      <c r="F51" s="3"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="2"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B52" s="6"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="3"/>
+      <c r="D52" s="2"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
+      <c r="F52" s="3"/>
       <c r="G52" s="4"/>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="2"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B53" s="6"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
+      <c r="D53" s="2"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
+      <c r="F53" s="3"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="2"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B54" s="6"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="3"/>
+      <c r="D54" s="2"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
+      <c r="F54" s="3"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="3"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="2"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B55" s="6"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
+      <c r="D55" s="2"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
+      <c r="F55" s="3"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="2"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B56" s="6"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
+      <c r="D56" s="2"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
+      <c r="F56" s="3"/>
       <c r="G56" s="4"/>
-      <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="2"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B57" s="6"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
+      <c r="D57" s="2"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
+      <c r="F57" s="3"/>
       <c r="G57" s="4"/>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="2"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B58" s="6"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="3"/>
+      <c r="D58" s="2"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="4"/>
+      <c r="F58" s="3"/>
       <c r="G58" s="4"/>
-      <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="2"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B59" s="6"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
+      <c r="D59" s="2"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
+      <c r="F59" s="3"/>
       <c r="G59" s="4"/>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="2"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B60" s="6"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
+      <c r="D60" s="2"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
+      <c r="F60" s="3"/>
       <c r="G60" s="4"/>
-      <c r="H60" s="3"/>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="2"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B61" s="6"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
+      <c r="D61" s="2"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
+      <c r="F61" s="3"/>
       <c r="G61" s="4"/>
-      <c r="H61" s="3"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="2"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="6"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="3"/>
+      <c r="D62" s="2"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
+      <c r="F62" s="3"/>
       <c r="G62" s="4"/>
-      <c r="H62" s="3"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="2"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63" s="6"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="3"/>
+      <c r="D63" s="2"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
+      <c r="F63" s="3"/>
       <c r="G63" s="4"/>
-      <c r="H63" s="3"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="2"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B64" s="6"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="3"/>
+      <c r="D64" s="2"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
+      <c r="F64" s="3"/>
       <c r="G64" s="4"/>
-      <c r="H64" s="3"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="2"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="6"/>
       <c r="C65" s="2"/>
-      <c r="D65" s="3"/>
+      <c r="D65" s="2"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
+      <c r="F65" s="3"/>
       <c r="G65" s="4"/>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="2"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="6"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="3"/>
+      <c r="D66" s="2"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
+      <c r="F66" s="3"/>
       <c r="G66" s="4"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="2"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B67" s="6"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="3"/>
+      <c r="D67" s="2"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
+      <c r="F67" s="3"/>
       <c r="G67" s="4"/>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="2"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="6"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="3"/>
+      <c r="D68" s="2"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
+      <c r="F68" s="3"/>
       <c r="G68" s="4"/>
-      <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="2"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B69" s="6"/>
       <c r="C69" s="2"/>
-      <c r="D69" s="3"/>
+      <c r="D69" s="2"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
+      <c r="F69" s="3"/>
       <c r="G69" s="4"/>
-      <c r="H69" s="3"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="2"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B70" s="6"/>
       <c r="C70" s="2"/>
-      <c r="D70" s="3"/>
+      <c r="D70" s="2"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
+      <c r="F70" s="3"/>
       <c r="G70" s="4"/>
-      <c r="H70" s="3"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="2"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B71" s="6"/>
       <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
+      <c r="D71" s="2"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
+      <c r="F71" s="3"/>
       <c r="G71" s="4"/>
-      <c r="H71" s="3"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="2"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B72" s="6"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="3"/>
+      <c r="D72" s="2"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
+      <c r="F72" s="3"/>
       <c r="G72" s="4"/>
-      <c r="H72" s="3"/>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="2"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B73" s="6"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="3"/>
+      <c r="D73" s="2"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
+      <c r="F73" s="3"/>
       <c r="G73" s="4"/>
-      <c r="H73" s="3"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="2"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B74" s="6"/>
       <c r="C74" s="2"/>
-      <c r="D74" s="3"/>
+      <c r="D74" s="2"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
+      <c r="F74" s="3"/>
       <c r="G74" s="4"/>
-      <c r="H74" s="3"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B75" s="2"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B75" s="6"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
+      <c r="D75" s="2"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
+      <c r="F75" s="3"/>
       <c r="G75" s="4"/>
-      <c r="H75" s="3"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="2"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B76" s="6"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
+      <c r="D76" s="2"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
+      <c r="F76" s="3"/>
       <c r="G76" s="4"/>
-      <c r="H76" s="3"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="2"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B77" s="6"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="3"/>
+      <c r="D77" s="2"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
+      <c r="F77" s="3"/>
       <c r="G77" s="4"/>
-      <c r="H77" s="3"/>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B78" s="2"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B78" s="6"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="3"/>
+      <c r="D78" s="2"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
+      <c r="F78" s="3"/>
       <c r="G78" s="4"/>
-      <c r="H78" s="3"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B79" s="2"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B79" s="6"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="3"/>
+      <c r="D79" s="2"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
+      <c r="F79" s="3"/>
       <c r="G79" s="4"/>
-      <c r="H79" s="3"/>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="2"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="6"/>
       <c r="C80" s="2"/>
-      <c r="D80" s="3"/>
+      <c r="D80" s="2"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
+      <c r="F80" s="3"/>
       <c r="G80" s="4"/>
-      <c r="H80" s="3"/>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B81" s="2"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81" s="6"/>
       <c r="C81" s="2"/>
-      <c r="D81" s="3"/>
+      <c r="D81" s="2"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
+      <c r="F81" s="3"/>
       <c r="G81" s="4"/>
-      <c r="H81" s="3"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B82" s="2"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B82" s="6"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="3"/>
+      <c r="D82" s="2"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
+      <c r="F82" s="3"/>
       <c r="G82" s="4"/>
-      <c r="H82" s="3"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="2"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="3"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B83" s="6"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="3"/>
+      <c r="D83" s="2"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
+      <c r="F83" s="3"/>
       <c r="G83" s="4"/>
-      <c r="H83" s="3"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="2"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="3"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B84" s="6"/>
       <c r="C84" s="2"/>
-      <c r="D84" s="3"/>
+      <c r="D84" s="2"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
+      <c r="F84" s="3"/>
       <c r="G84" s="4"/>
-      <c r="H84" s="3"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="2"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="3"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B85" s="6"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="3"/>
+      <c r="D85" s="2"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
+      <c r="F85" s="3"/>
       <c r="G85" s="4"/>
-      <c r="H85" s="3"/>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B86" s="2"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="3"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B86" s="6"/>
       <c r="C86" s="2"/>
-      <c r="D86" s="3"/>
+      <c r="D86" s="2"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
+      <c r="F86" s="3"/>
       <c r="G86" s="4"/>
-      <c r="H86" s="3"/>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B87" s="2"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="3"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B87" s="6"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="3"/>
+      <c r="D87" s="2"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
+      <c r="F87" s="3"/>
       <c r="G87" s="4"/>
-      <c r="H87" s="3"/>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B88" s="2"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="3"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B88" s="6"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="3"/>
+      <c r="D88" s="2"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
+      <c r="F88" s="3"/>
       <c r="G88" s="4"/>
-      <c r="H88" s="3"/>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B89" s="2"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="3"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B89" s="6"/>
       <c r="C89" s="2"/>
-      <c r="D89" s="3"/>
+      <c r="D89" s="2"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
+      <c r="F89" s="3"/>
       <c r="G89" s="4"/>
-      <c r="H89" s="3"/>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B90" s="2"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="3"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B90" s="6"/>
       <c r="C90" s="2"/>
-      <c r="D90" s="3"/>
+      <c r="D90" s="2"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
+      <c r="F90" s="3"/>
       <c r="G90" s="4"/>
-      <c r="H90" s="3"/>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B91" s="2"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="3"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B91" s="6"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="3"/>
+      <c r="D91" s="2"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
+      <c r="F91" s="3"/>
       <c r="G91" s="4"/>
-      <c r="H91" s="3"/>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B92" s="2"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="3"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B92" s="6"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="3"/>
+      <c r="D92" s="2"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
+      <c r="F92" s="3"/>
       <c r="G92" s="4"/>
-      <c r="H92" s="3"/>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B93" s="2"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="3"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B93" s="6"/>
       <c r="C93" s="2"/>
-      <c r="D93" s="3"/>
+      <c r="D93" s="2"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
+      <c r="F93" s="3"/>
       <c r="G93" s="4"/>
-      <c r="H93" s="3"/>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B94" s="2"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="3"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B94" s="6"/>
       <c r="C94" s="2"/>
-      <c r="D94" s="3"/>
+      <c r="D94" s="2"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
+      <c r="F94" s="3"/>
       <c r="G94" s="4"/>
-      <c r="H94" s="3"/>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B95" s="2"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="3"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B95" s="6"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="3"/>
+      <c r="D95" s="2"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
+      <c r="F95" s="3"/>
       <c r="G95" s="4"/>
-      <c r="H95" s="3"/>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B96" s="2"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="3"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B96" s="6"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="3"/>
+      <c r="D96" s="2"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
+      <c r="F96" s="3"/>
       <c r="G96" s="4"/>
-      <c r="H96" s="3"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B97" s="2"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="3"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B97" s="6"/>
       <c r="C97" s="2"/>
-      <c r="D97" s="3"/>
+      <c r="D97" s="2"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
+      <c r="F97" s="3"/>
       <c r="G97" s="4"/>
-      <c r="H97" s="3"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B98" s="2"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="3"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B98" s="6"/>
       <c r="C98" s="2"/>
-      <c r="D98" s="3"/>
+      <c r="D98" s="2"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
+      <c r="F98" s="3"/>
       <c r="G98" s="4"/>
-      <c r="H98" s="3"/>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B99" s="2"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="3"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B99" s="6"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="3"/>
+      <c r="D99" s="2"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
+      <c r="F99" s="3"/>
       <c r="G99" s="4"/>
-      <c r="H99" s="3"/>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B100" s="2"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="3"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B100" s="6"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="3"/>
+      <c r="D100" s="2"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
+      <c r="F100" s="3"/>
       <c r="G100" s="4"/>
-      <c r="H100" s="3"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:C25">
+  <autoFilter ref="C2:D25">
     <filterColumn colId="1">
       <filters>
         <filter val="To do"/>
@@ -1885,41 +2027,41 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="B3:H28">
-    <sortCondition sortBy="cellColor" ref="B3:B28" dxfId="8"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="B3:B28" dxfId="7"/>
+  <sortState ref="C3:I28">
+    <sortCondition sortBy="cellColor" ref="C3:C28" dxfId="10"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C28" dxfId="9"/>
   </sortState>
-  <conditionalFormatting sqref="B3:B100">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+  <conditionalFormatting sqref="C3:C100">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C100">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="D3:D100">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="C3:C100">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D3:D100">
       <formula1>"To do,In progress,To test,Done"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="B3:B100">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="C3:C100">
       <formula1>"High,Medium,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Works.xlsx : Add a new functionnalities.
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$C$2:$D$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$C$2:$D$29</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Priority</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>to show the color's signification</t>
+  </si>
+  <si>
+    <t>to implement the comment in XML file (rules coloring)</t>
   </si>
 </sst>
 </file>
@@ -298,7 +304,23 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -681,7 +703,7 @@
   <dimension ref="B2:I100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -773,6 +795,10 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="6">
+        <f>ROW()</f>
+        <v>5</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -794,6 +820,10 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="6">
+        <f>ROW()</f>
+        <v>6</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
@@ -815,6 +845,10 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6">
+        <f>ROW()</f>
+        <v>7</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -836,6 +870,10 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6">
+        <f>ROW()</f>
+        <v>8</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
@@ -857,6 +895,10 @@
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <f>ROW()</f>
+        <v>9</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
@@ -878,6 +920,10 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
+        <f>ROW()</f>
+        <v>10</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
@@ -899,6 +945,10 @@
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6">
+        <f>ROW()</f>
+        <v>11</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
@@ -920,6 +970,10 @@
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6">
+        <f>ROW()</f>
+        <v>12</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
@@ -941,6 +995,10 @@
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6">
+        <f>ROW()</f>
+        <v>13</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
@@ -962,6 +1020,10 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6">
+        <f>ROW()</f>
+        <v>14</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1033,6 +1095,10 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6">
+        <f>ROW()</f>
+        <v>17</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1054,6 +1120,10 @@
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6">
+        <f>ROW()</f>
+        <v>18</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1075,6 +1145,10 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6">
+        <f>ROW()</f>
+        <v>19</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1096,6 +1170,10 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6">
+        <f>ROW()</f>
+        <v>20</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1186,6 +1264,10 @@
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6">
+        <f>ROW()</f>
+        <v>24</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1235,19 +1317,19 @@
         <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G26" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
@@ -1264,13 +1346,13 @@
         <v>39</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G27" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
@@ -1287,24 +1369,37 @@
         <v>39</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G28" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="6"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="6">
+        <f>ROW()</f>
+        <v>29</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
@@ -2019,7 +2114,7 @@
       <c r="I100" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:D25">
+  <autoFilter ref="C2:D29">
     <filterColumn colId="1">
       <filters>
         <filter val="To do"/>
@@ -2027,32 +2122,32 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="C3:I28">
-    <sortCondition sortBy="cellColor" ref="C3:C28" dxfId="10"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C28" dxfId="9"/>
+  <sortState ref="B3:I29">
+    <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="3"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="2"/>
   </sortState>
   <conditionalFormatting sqref="C3:C100">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D100">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ticket #9 and ID 26 : Implementing comment from XML rule file The comment is read and displayed on hovered value
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -282,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +298,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,7 +706,7 @@
   <dimension ref="B2:I100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1069,7 +1072,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6">
         <f>ROW()</f>
         <v>16</v>
@@ -1078,7 +1081,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>54</v>
@@ -1320,7 +1323,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>67</v>
@@ -1331,7 +1334,9 @@
       <c r="G26" s="4">
         <v>2</v>
       </c>
-      <c r="H26" s="4"/>
+      <c r="H26" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ticket #6 and ID 25 : Implementing saving automatically VSObserver can create and write the locked list
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
   <si>
     <t>Priority</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>to implement the comment in XML file (rules coloring)</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -307,39 +310,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -706,7 +677,7 @@
   <dimension ref="B2:I100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1047,7 +1018,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <f>ROW()</f>
         <v>15</v>
@@ -1056,7 +1027,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>44</v>
@@ -1300,7 +1271,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>59</v>
@@ -2128,31 +2099,31 @@
     </filterColumn>
   </autoFilter>
   <sortState ref="B3:I29">
-    <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="3"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="8"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="7"/>
   </sortState>
   <conditionalFormatting sqref="C3:C100">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D100">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ticket #6 and ID 25 : Locked variables are automatically saved and loaded The CSV file containing all locked variables is loaded in starting of VSObserver
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Priority</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>to implement the comment in XML file (rules coloring)</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -677,7 +674,7 @@
   <dimension ref="B2:I100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1271,7 +1268,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
ID 23 and associated to ticket #7: The height isn't changing anymore Now a bubble appears at left of search field. This bubble shows the error when we put the mouse over the bubble.
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$C$2:$D$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$C$2:$D$28</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>Priority</t>
   </si>
@@ -188,12 +188,6 @@
     <t>to display the good value or wrong value direclty in background</t>
   </si>
   <si>
-    <t>to set a search background color when the regex is wrong or good</t>
-  </si>
-  <si>
-    <t>to see whether the regex has worked</t>
-  </si>
-  <si>
     <t>Real (hours)</t>
   </si>
   <si>
@@ -203,12 +197,6 @@
     <t>to load automatically the locked list and the application shouldn't carsh</t>
   </si>
   <si>
-    <t>to display the information in a status bar</t>
-  </si>
-  <si>
-    <t>for the messages doesn't alter the size</t>
-  </si>
-  <si>
     <t>to save as a list of locked variable</t>
   </si>
   <si>
@@ -222,6 +210,12 @@
   </si>
   <si>
     <t>to implement the comment in XML file (rules coloring)</t>
+  </si>
+  <si>
+    <t>to set a bubble to advertise the users</t>
+  </si>
+  <si>
+    <t>to see whether there is a error on search</t>
   </si>
 </sst>
 </file>
@@ -671,10 +665,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1" filterMode="1"/>
-  <dimension ref="B2:I100"/>
+  <dimension ref="B2:I99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -691,7 +685,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -709,7 +703,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>5</v>
@@ -1220,18 +1214,20 @@
         <v>14</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G23" s="4">
         <v>1</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="4">
+        <v>1</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1271,15 +1267,17 @@
         <v>34</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G25" s="4">
         <v>3</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
@@ -1294,10 +1292,10 @@
         <v>34</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G26" s="4">
         <v>2</v>
@@ -1342,37 +1340,24 @@
         <v>39</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G28" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="6">
-        <f>ROW()</f>
-        <v>29</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="4">
-        <v>3</v>
-      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
@@ -2076,18 +2061,8 @@
       <c r="H99" s="4"/>
       <c r="I99" s="3"/>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B100" s="6"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="C2:D29">
+  <autoFilter ref="C2:D28">
     <filterColumn colId="1">
       <filters>
         <filter val="To do"/>
@@ -2099,7 +2074,7 @@
     <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="8"/>
     <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="7"/>
   </sortState>
-  <conditionalFormatting sqref="C3:C100">
+  <conditionalFormatting sqref="C3:C99">
     <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
@@ -2110,7 +2085,7 @@
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D100">
+  <conditionalFormatting sqref="D3:D99">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
@@ -2125,11 +2100,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D3:D100">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D3:D99">
       <formula1>"To do,In progress,To test,Done"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="C3:C100">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="C3:C99">
       <formula1>"High,Medium,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
ID 22: We can copy directly the name and path of variable. The path and name of variable is copied when the variable is copied (ctrl + c)
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -668,7 +668,7 @@
   <dimension ref="B2:I99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1191,7 +1191,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>52</v>
@@ -1202,7 +1202,9 @@
       <c r="G22" s="4">
         <v>2</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="7">
+        <v>6.25E-2</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Offline mode to get all variables: When VSObserver don't get to connect to the U-Test server, the tools sent back zero variables founded. Now VSObserver browses the SQLite database to get all variables. The tool do that only it don't get to connect to U-Test server.
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Priority</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>to see whether there is a error on search</t>
+  </si>
+  <si>
+    <t>Improve search and refresh</t>
+  </si>
+  <si>
+    <t>to more fluidity and avoid undefined variables</t>
   </si>
 </sst>
 </file>
@@ -301,7 +307,39 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -668,7 +706,7 @@
   <dimension ref="B2:I99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1165,16 +1203,16 @@
         <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="G21" s="4">
         <v>4</v>
@@ -1182,7 +1220,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <f>ROW()</f>
         <v>22</v>
@@ -1191,7 +1229,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>52</v>
@@ -1216,20 +1254,18 @@
         <v>14</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G23" s="4">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1257,7 +1293,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <f>ROW()</f>
         <v>25</v>
@@ -1266,7 +1302,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>57</v>
@@ -1282,7 +1318,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <f>ROW()</f>
         <v>26</v>
@@ -1291,7 +1327,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>63</v>
@@ -1313,21 +1349,23 @@
         <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="G27" s="4">
-        <v>4</v>
-      </c>
-      <c r="H27" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
@@ -1342,24 +1380,37 @@
         <v>39</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G28" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="6"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="6">
+        <f>ROW()</f>
+        <v>29</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
@@ -2073,31 +2124,31 @@
     </filterColumn>
   </autoFilter>
   <sortState ref="B3:I29">
-    <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="8"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="7"/>
+    <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="3"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="2"/>
   </sortState>
   <conditionalFormatting sqref="C3:C99">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D99">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ticket #8 and ID #29 : Locked list Add the button with context menu
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
   <si>
     <t>Priority</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>to more fluidity and avoid undefined variables</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -307,39 +310,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -706,7 +677,7 @@
   <dimension ref="B2:I99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1400,7 +1371,7 @@
         <v>11</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>59</v>
@@ -2124,31 +2095,31 @@
     </filterColumn>
   </autoFilter>
   <sortState ref="B3:I29">
-    <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="3"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="8"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="7"/>
   </sortState>
   <conditionalFormatting sqref="C3:C99">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D99">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"To test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ticket #8 and ID #29 : Saving locked list Loading of saved locked list is implemented. This function is finished at this state
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Priority</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>to more fluidity and avoid undefined variables</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -677,7 +674,7 @@
   <dimension ref="B2:I99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1371,7 +1368,7 @@
         <v>11</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
ID #30 : Remove "hide" button The "hide" button has been removed. Now, the window appears when it has been minimized
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Feuille2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$C$2:$D$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$C$2:$D$30</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>Priority</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>to more fluidity and avoid undefined variables</t>
+  </si>
+  <si>
+    <t>to remove the hide button</t>
+  </si>
+  <si>
+    <t>instead make visible the windows when it has been minimized</t>
   </si>
 </sst>
 </file>
@@ -674,7 +680,7 @@
   <dimension ref="B2:I99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1379,17 +1385,34 @@
       <c r="G29" s="4">
         <v>3</v>
       </c>
-      <c r="H29" s="4"/>
+      <c r="H29" s="4">
+        <v>4</v>
+      </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="6"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+    <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6">
+        <f>ROW()</f>
+        <v>30</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H30" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
@@ -2083,7 +2106,7 @@
       <c r="I99" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:D28">
+  <autoFilter ref="C2:D30">
     <filterColumn colId="1">
       <filters>
         <filter val="To do"/>

</xml_diff>

<commit_message>
Works : Add some functionalities
</commit_message>
<xml_diff>
--- a/Works.xlsx
+++ b/Works.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>Priority</t>
   </si>
@@ -228,13 +228,16 @@
   </si>
   <si>
     <t>instead make visible the windows when it has been minimized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add variable in parameters file from VSObserver </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -249,6 +252,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -285,10 +295,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,8 +320,10 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -676,11 +689,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuil1" filterMode="1"/>
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="B2:I99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -771,7 +784,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="6">
         <f>ROW()</f>
         <v>5</v>
@@ -796,7 +809,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="6">
         <f>ROW()</f>
         <v>6</v>
@@ -821,7 +834,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="6">
         <f>ROW()</f>
         <v>7</v>
@@ -846,7 +859,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <f>ROW()</f>
         <v>8</v>
@@ -871,7 +884,7 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="6">
         <f>ROW()</f>
         <v>9</v>
@@ -896,7 +909,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
         <f>ROW()</f>
         <v>10</v>
@@ -921,7 +934,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="6">
         <f>ROW()</f>
         <v>11</v>
@@ -946,7 +959,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <f>ROW()</f>
         <v>12</v>
@@ -971,7 +984,7 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <f>ROW()</f>
         <v>13</v>
@@ -996,7 +1009,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <f>ROW()</f>
         <v>14</v>
@@ -1021,7 +1034,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <f>ROW()</f>
         <v>15</v>
@@ -1046,7 +1059,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="6">
         <f>ROW()</f>
         <v>16</v>
@@ -1071,7 +1084,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <f>ROW()</f>
         <v>17</v>
@@ -1096,7 +1109,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <f>ROW()</f>
         <v>18</v>
@@ -1121,7 +1134,7 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="6">
         <f>ROW()</f>
         <v>19</v>
@@ -1146,7 +1159,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <f>ROW()</f>
         <v>20</v>
@@ -1180,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>66</v>
@@ -1191,10 +1204,12 @@
       <c r="G21" s="4">
         <v>4</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4">
+        <v>8</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <f>ROW()</f>
         <v>22</v>
@@ -1242,7 +1257,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="6">
         <f>ROW()</f>
         <v>24</v>
@@ -1267,7 +1282,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <f>ROW()</f>
         <v>25</v>
@@ -1292,7 +1307,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <f>ROW()</f>
         <v>26</v>
@@ -1326,7 +1341,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>64</v>
@@ -1351,7 +1366,7 @@
         <v>11</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>46</v>
@@ -1362,7 +1377,9 @@
       <c r="G28" s="4">
         <v>4</v>
       </c>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4">
+        <v>8</v>
+      </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
@@ -1374,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>59</v>
@@ -1390,7 +1407,7 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
         <f>ROW()</f>
         <v>30</v>
@@ -1416,13 +1433,25 @@
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="6"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
+      <c r="B31" s="6">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="G31" s="4">
+        <v>10</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0.4375</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
@@ -2106,14 +2135,7 @@
       <c r="I99" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:D30">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="To do"/>
-        <filter val="To test"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C2:D30"/>
   <sortState ref="B3:I29">
     <sortCondition sortBy="cellColor" ref="C3:C29" dxfId="8"/>
     <sortCondition descending="1" sortBy="cellColor" ref="C3:C29" dxfId="7"/>
@@ -2153,8 +2175,11 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E31" r:id="rId1" display="https://github.com/Edwix/VSObserver/issues/12"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>